<commit_message>
update OverTime Model for EF Core
</commit_message>
<xml_diff>
--- a/wwwroot/reports/PaperTaskMachine2.xlsx
+++ b/wwwroot/reports/PaperTaskMachine2.xlsx
@@ -464,6 +464,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,9 +484,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
@@ -1242,34 +1242,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="55.8" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="41"/>
     </row>
     <row r="2" spans="1:11" ht="21.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="44"/>
     </row>
     <row r="3" spans="1:11" ht="21.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2"/>
@@ -1360,7 +1360,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="38" t="s">
         <v>43</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -1513,19 +1513,19 @@
       <c r="K18" s="35"/>
     </row>
     <row r="19" spans="1:11" ht="21.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="44"/>
     </row>
     <row r="20" spans="1:11" ht="22.2" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A20" s="24"/>
@@ -1534,13 +1534,13 @@
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I20" s="32" t="s">
+      <c r="H20" s="32" t="s">
         <v>30</v>
       </c>
+      <c r="I20" s="32"/>
       <c r="J20" s="14"/>
       <c r="K20" s="33"/>
     </row>

</xml_diff>